<commit_message>
Se carga un mapa de csv
</commit_message>
<xml_diff>
--- a/assets/mapa1-editable.xlsx
+++ b/assets/mapa1-editable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\MultiAgentes\NatureEngine\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BA837A9-2B5E-42FB-A7FA-21DB12A5FA43}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B6487F-66BE-4DE2-9AFF-68C184D89D15}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{42A3EED4-75C0-43E2-B9DC-769AA40C7AF2}"/>
   </bookViews>
@@ -75,9 +75,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,8 +403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CE728B6-19BC-4F2E-8578-ED7E7A650263}">
   <dimension ref="A1:CL179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B54" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="CH80" sqref="CH80"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V92" sqref="V92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24095,365 +24096,817 @@
       <c r="A90" s="1">
         <v>0</v>
       </c>
-      <c r="B90" s="1">
-        <v>0</v>
-      </c>
-      <c r="C90" s="1">
-        <v>0</v>
-      </c>
-      <c r="D90" s="1">
-        <v>0</v>
-      </c>
-      <c r="E90" s="1">
-        <v>0</v>
-      </c>
-      <c r="F90" s="1">
-        <v>0</v>
-      </c>
-      <c r="G90" s="1">
-        <v>0</v>
-      </c>
-      <c r="H90" s="1">
-        <v>0</v>
-      </c>
-      <c r="I90" s="1">
-        <v>0</v>
-      </c>
-      <c r="J90" s="1">
-        <v>0</v>
-      </c>
-      <c r="K90" s="1">
-        <v>0</v>
-      </c>
-      <c r="L90" s="1">
-        <v>0</v>
-      </c>
-      <c r="M90" s="1">
-        <v>0</v>
-      </c>
-      <c r="N90" s="1">
-        <v>0</v>
-      </c>
-      <c r="O90" s="1">
-        <v>0</v>
-      </c>
-      <c r="P90" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q90" s="1">
-        <v>0</v>
-      </c>
-      <c r="R90" s="1">
-        <v>0</v>
-      </c>
-      <c r="S90" s="1">
-        <v>0</v>
-      </c>
-      <c r="T90" s="1">
-        <v>0</v>
-      </c>
-      <c r="U90" s="1">
-        <v>0</v>
-      </c>
-      <c r="V90" s="1">
-        <v>0</v>
-      </c>
-      <c r="W90" s="1">
-        <v>0</v>
-      </c>
-      <c r="X90" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y90" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AF90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AK90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AL90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AM90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AN90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AO90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AP90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AQ90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AS90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AT90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AU90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AW90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AX90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AY90" s="1">
-        <v>0</v>
-      </c>
-      <c r="AZ90" s="1">
-        <v>0</v>
-      </c>
-      <c r="BA90" s="1">
-        <v>0</v>
-      </c>
-      <c r="BB90" s="1">
-        <v>0</v>
-      </c>
-      <c r="BC90" s="1">
-        <v>0</v>
-      </c>
-      <c r="BD90" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE90" s="1">
-        <v>0</v>
-      </c>
-      <c r="BF90" s="1">
-        <v>0</v>
-      </c>
-      <c r="BG90" s="1">
-        <v>0</v>
-      </c>
-      <c r="BH90" s="1">
-        <v>0</v>
-      </c>
-      <c r="BI90" s="1">
-        <v>0</v>
-      </c>
-      <c r="BJ90" s="1">
-        <v>0</v>
-      </c>
-      <c r="BK90" s="1">
-        <v>0</v>
-      </c>
-      <c r="BL90" s="1">
-        <v>0</v>
-      </c>
-      <c r="BM90" s="1">
-        <v>0</v>
-      </c>
-      <c r="BN90" s="1">
-        <v>0</v>
-      </c>
-      <c r="BO90" s="1">
-        <v>0</v>
-      </c>
-      <c r="BP90" s="1">
-        <v>0</v>
-      </c>
-      <c r="BQ90" s="1">
-        <v>0</v>
-      </c>
-      <c r="BR90" s="1">
-        <v>0</v>
-      </c>
-      <c r="BS90" s="1">
-        <v>0</v>
-      </c>
-      <c r="BT90" s="1">
-        <v>0</v>
-      </c>
-      <c r="BU90" s="1">
-        <v>0</v>
-      </c>
-      <c r="BV90" s="1">
-        <v>0</v>
-      </c>
-      <c r="BW90" s="1">
-        <v>0</v>
-      </c>
-      <c r="BX90" s="1">
-        <v>0</v>
-      </c>
-      <c r="BY90" s="1">
-        <v>0</v>
-      </c>
-      <c r="BZ90" s="1">
-        <v>0</v>
-      </c>
-      <c r="CA90" s="1">
-        <v>0</v>
-      </c>
-      <c r="CB90" s="1">
-        <v>0</v>
-      </c>
-      <c r="CC90" s="1">
-        <v>0</v>
-      </c>
-      <c r="CD90" s="1">
-        <v>0</v>
-      </c>
-      <c r="CE90" s="1">
-        <v>0</v>
-      </c>
-      <c r="CF90" s="1">
-        <v>0</v>
-      </c>
-      <c r="CG90" s="1">
-        <v>0</v>
-      </c>
-      <c r="CH90" s="1">
-        <v>0</v>
-      </c>
-      <c r="CI90" s="1">
-        <v>0</v>
-      </c>
-      <c r="CJ90" s="1">
-        <v>0</v>
-      </c>
-      <c r="CK90" s="1">
-        <v>0</v>
-      </c>
-      <c r="CL90" s="1">
+      <c r="B90" s="2">
+        <v>0</v>
+      </c>
+      <c r="C90" s="2">
+        <v>0</v>
+      </c>
+      <c r="D90" s="2">
+        <v>0</v>
+      </c>
+      <c r="E90" s="2">
+        <v>0</v>
+      </c>
+      <c r="F90" s="2">
+        <v>0</v>
+      </c>
+      <c r="G90" s="2">
+        <v>0</v>
+      </c>
+      <c r="H90" s="2">
+        <v>0</v>
+      </c>
+      <c r="I90" s="2">
+        <v>0</v>
+      </c>
+      <c r="J90" s="2">
+        <v>0</v>
+      </c>
+      <c r="K90" s="2">
+        <v>0</v>
+      </c>
+      <c r="L90" s="2">
+        <v>0</v>
+      </c>
+      <c r="M90" s="2">
+        <v>0</v>
+      </c>
+      <c r="N90" s="2">
+        <v>0</v>
+      </c>
+      <c r="O90" s="2">
+        <v>0</v>
+      </c>
+      <c r="P90" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q90" s="2">
+        <v>0</v>
+      </c>
+      <c r="R90" s="2">
+        <v>0</v>
+      </c>
+      <c r="S90" s="2">
+        <v>0</v>
+      </c>
+      <c r="T90" s="2">
+        <v>0</v>
+      </c>
+      <c r="U90" s="2">
+        <v>0</v>
+      </c>
+      <c r="V90" s="2">
+        <v>0</v>
+      </c>
+      <c r="W90" s="2">
+        <v>0</v>
+      </c>
+      <c r="X90" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y90" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z90" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA90" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB90" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC90" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD90" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE90" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF90" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG90" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH90" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI90" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ90" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK90" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL90" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM90" s="2">
+        <v>0</v>
+      </c>
+      <c r="AN90" s="2">
+        <v>0</v>
+      </c>
+      <c r="AO90" s="2">
+        <v>0</v>
+      </c>
+      <c r="AP90" s="2">
+        <v>0</v>
+      </c>
+      <c r="AQ90" s="2">
+        <v>0</v>
+      </c>
+      <c r="AR90" s="2">
+        <v>0</v>
+      </c>
+      <c r="AS90" s="2">
+        <v>0</v>
+      </c>
+      <c r="AT90" s="2">
+        <v>0</v>
+      </c>
+      <c r="AU90" s="2">
+        <v>0</v>
+      </c>
+      <c r="AV90" s="2">
+        <v>0</v>
+      </c>
+      <c r="AW90" s="2">
+        <v>0</v>
+      </c>
+      <c r="AX90" s="2">
+        <v>0</v>
+      </c>
+      <c r="AY90" s="2">
+        <v>0</v>
+      </c>
+      <c r="AZ90" s="2">
+        <v>0</v>
+      </c>
+      <c r="BA90" s="2">
+        <v>0</v>
+      </c>
+      <c r="BB90" s="2">
+        <v>0</v>
+      </c>
+      <c r="BC90" s="2">
+        <v>0</v>
+      </c>
+      <c r="BD90" s="2">
+        <v>0</v>
+      </c>
+      <c r="BE90" s="2">
+        <v>0</v>
+      </c>
+      <c r="BF90" s="2">
+        <v>0</v>
+      </c>
+      <c r="BG90" s="2">
+        <v>0</v>
+      </c>
+      <c r="BH90" s="2">
+        <v>0</v>
+      </c>
+      <c r="BI90" s="2">
+        <v>0</v>
+      </c>
+      <c r="BJ90" s="2">
+        <v>0</v>
+      </c>
+      <c r="BK90" s="2">
+        <v>0</v>
+      </c>
+      <c r="BL90" s="2">
+        <v>0</v>
+      </c>
+      <c r="BM90" s="2">
+        <v>0</v>
+      </c>
+      <c r="BN90" s="2">
+        <v>0</v>
+      </c>
+      <c r="BO90" s="2">
+        <v>0</v>
+      </c>
+      <c r="BP90" s="2">
+        <v>0</v>
+      </c>
+      <c r="BQ90" s="2">
+        <v>0</v>
+      </c>
+      <c r="BR90" s="2">
+        <v>0</v>
+      </c>
+      <c r="BS90" s="2">
+        <v>0</v>
+      </c>
+      <c r="BT90" s="2">
+        <v>0</v>
+      </c>
+      <c r="BU90" s="2">
+        <v>0</v>
+      </c>
+      <c r="BV90" s="2">
+        <v>0</v>
+      </c>
+      <c r="BW90" s="2">
+        <v>0</v>
+      </c>
+      <c r="BX90" s="2">
+        <v>0</v>
+      </c>
+      <c r="BY90" s="2">
+        <v>0</v>
+      </c>
+      <c r="BZ90" s="2">
+        <v>0</v>
+      </c>
+      <c r="CA90" s="2">
+        <v>0</v>
+      </c>
+      <c r="CB90" s="2">
+        <v>0</v>
+      </c>
+      <c r="CC90" s="2">
+        <v>0</v>
+      </c>
+      <c r="CD90" s="2">
+        <v>0</v>
+      </c>
+      <c r="CE90" s="2">
+        <v>0</v>
+      </c>
+      <c r="CF90" s="2">
+        <v>0</v>
+      </c>
+      <c r="CG90" s="2">
+        <v>0</v>
+      </c>
+      <c r="CH90" s="2">
+        <v>0</v>
+      </c>
+      <c r="CI90" s="2">
+        <v>0</v>
+      </c>
+      <c r="CJ90" s="2">
+        <v>0</v>
+      </c>
+      <c r="CK90" s="2">
+        <v>0</v>
+      </c>
+      <c r="CL90" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:90" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>0</v>
+      </c>
+      <c r="B91" s="2">
+        <v>0</v>
+      </c>
+      <c r="C91" s="2">
+        <v>0</v>
+      </c>
+      <c r="D91" s="2">
+        <v>0</v>
+      </c>
+      <c r="E91" s="2">
+        <v>0</v>
+      </c>
+      <c r="F91" s="2">
+        <v>0</v>
+      </c>
+      <c r="G91" s="2">
+        <v>0</v>
+      </c>
+      <c r="H91" s="2">
+        <v>0</v>
+      </c>
+      <c r="I91" s="2">
+        <v>0</v>
+      </c>
+      <c r="J91" s="2">
+        <v>0</v>
+      </c>
+      <c r="K91" s="2">
+        <v>0</v>
+      </c>
+      <c r="L91" s="2">
+        <v>0</v>
+      </c>
+      <c r="M91" s="2">
+        <v>0</v>
+      </c>
+      <c r="N91" s="2">
+        <v>0</v>
+      </c>
+      <c r="O91" s="2">
+        <v>0</v>
+      </c>
+      <c r="P91" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q91" s="2">
+        <v>0</v>
+      </c>
+      <c r="R91" s="2">
+        <v>0</v>
+      </c>
+      <c r="S91" s="2">
+        <v>0</v>
+      </c>
+      <c r="T91" s="2">
+        <v>0</v>
+      </c>
+      <c r="U91" s="2">
+        <v>0</v>
+      </c>
+      <c r="V91" s="2">
+        <v>0</v>
+      </c>
+      <c r="W91" s="2">
+        <v>0</v>
+      </c>
+      <c r="X91" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y91" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z91" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA91" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB91" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC91" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD91" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE91" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF91" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG91" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH91" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI91" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ91" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK91" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL91" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM91" s="2">
+        <v>0</v>
+      </c>
+      <c r="AN91" s="2">
+        <v>0</v>
+      </c>
+      <c r="AO91" s="2">
+        <v>0</v>
+      </c>
+      <c r="AP91" s="2">
+        <v>0</v>
+      </c>
+      <c r="AQ91" s="2">
+        <v>0</v>
+      </c>
+      <c r="AR91" s="2">
+        <v>0</v>
+      </c>
+      <c r="AS91" s="2">
+        <v>0</v>
+      </c>
+      <c r="AT91" s="2">
+        <v>0</v>
+      </c>
+      <c r="AU91" s="2">
+        <v>0</v>
+      </c>
+      <c r="AV91" s="2">
+        <v>0</v>
+      </c>
+      <c r="AW91" s="2">
+        <v>0</v>
+      </c>
+      <c r="AX91" s="2">
+        <v>0</v>
+      </c>
+      <c r="AY91" s="2">
+        <v>0</v>
+      </c>
+      <c r="AZ91" s="2">
+        <v>0</v>
+      </c>
+      <c r="BA91" s="2">
+        <v>0</v>
+      </c>
+      <c r="BB91" s="2">
+        <v>0</v>
+      </c>
+      <c r="BC91" s="2">
+        <v>0</v>
+      </c>
+      <c r="BD91" s="2">
+        <v>0</v>
+      </c>
+      <c r="BE91" s="2">
+        <v>0</v>
+      </c>
+      <c r="BF91" s="2">
+        <v>0</v>
+      </c>
+      <c r="BG91" s="2">
+        <v>0</v>
+      </c>
+      <c r="BH91" s="2">
+        <v>0</v>
+      </c>
+      <c r="BI91" s="2">
+        <v>0</v>
+      </c>
+      <c r="BJ91" s="2">
+        <v>0</v>
+      </c>
+      <c r="BK91" s="2">
+        <v>0</v>
+      </c>
+      <c r="BL91" s="2">
+        <v>0</v>
+      </c>
+      <c r="BM91" s="2">
+        <v>0</v>
+      </c>
+      <c r="BN91" s="2">
+        <v>0</v>
+      </c>
+      <c r="BO91" s="2">
+        <v>0</v>
+      </c>
+      <c r="BP91" s="2">
+        <v>0</v>
+      </c>
+      <c r="BQ91" s="2">
+        <v>0</v>
+      </c>
+      <c r="BR91" s="2">
+        <v>0</v>
+      </c>
+      <c r="BS91" s="2">
+        <v>0</v>
+      </c>
+      <c r="BT91" s="2">
+        <v>0</v>
+      </c>
+      <c r="BU91" s="2">
+        <v>0</v>
+      </c>
+      <c r="BV91" s="2">
+        <v>0</v>
+      </c>
+      <c r="BW91" s="2">
+        <v>0</v>
+      </c>
+      <c r="BX91" s="2">
+        <v>0</v>
+      </c>
+      <c r="BY91" s="2">
+        <v>0</v>
+      </c>
+      <c r="BZ91" s="2">
+        <v>0</v>
+      </c>
+      <c r="CA91" s="2">
+        <v>0</v>
+      </c>
+      <c r="CB91" s="2">
+        <v>0</v>
+      </c>
+      <c r="CC91" s="2">
+        <v>0</v>
+      </c>
+      <c r="CD91" s="2">
+        <v>0</v>
+      </c>
+      <c r="CE91" s="2">
+        <v>0</v>
+      </c>
+      <c r="CF91" s="2">
+        <v>0</v>
+      </c>
+      <c r="CG91" s="2">
+        <v>0</v>
+      </c>
+      <c r="CH91" s="2">
+        <v>0</v>
+      </c>
+      <c r="CI91" s="2">
+        <v>0</v>
+      </c>
+      <c r="CJ91" s="2">
+        <v>0</v>
+      </c>
+      <c r="CK91" s="2">
+        <v>0</v>
+      </c>
+      <c r="CL91" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:90" x14ac:dyDescent="0.25">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
-      <c r="C92" s="1"/>
-      <c r="D92" s="1"/>
-      <c r="E92" s="1"/>
-      <c r="F92" s="1"/>
-      <c r="G92" s="1"/>
-      <c r="H92" s="1"/>
-      <c r="I92" s="1"/>
-      <c r="J92" s="1"/>
-      <c r="K92" s="1"/>
-      <c r="L92" s="1"/>
-      <c r="M92" s="1"/>
-      <c r="N92" s="1"/>
-      <c r="O92" s="1"/>
-      <c r="P92" s="1"/>
-      <c r="Q92" s="1"/>
-      <c r="R92" s="1"/>
-      <c r="S92" s="1"/>
-      <c r="T92" s="1"/>
-      <c r="U92" s="1"/>
-      <c r="V92" s="1"/>
-      <c r="W92" s="1"/>
-      <c r="X92" s="1"/>
-      <c r="Y92" s="1"/>
-      <c r="Z92" s="1"/>
-      <c r="AA92" s="1"/>
-      <c r="AB92" s="1"/>
-      <c r="AC92" s="1"/>
-      <c r="AD92" s="1"/>
-      <c r="AE92" s="1"/>
-      <c r="AF92" s="1"/>
-      <c r="AG92" s="1"/>
-      <c r="AH92" s="1"/>
-      <c r="AI92" s="1"/>
-      <c r="AJ92" s="1"/>
-      <c r="AK92" s="1"/>
-      <c r="AL92" s="1"/>
-      <c r="AM92" s="1"/>
-      <c r="AN92" s="1"/>
-      <c r="AO92" s="1"/>
-      <c r="AP92" s="1"/>
-      <c r="AQ92" s="1"/>
-      <c r="AR92" s="1"/>
-      <c r="AS92" s="1"/>
-      <c r="AT92" s="1"/>
-      <c r="AU92" s="1"/>
-      <c r="AV92" s="1"/>
-      <c r="AW92" s="1"/>
-      <c r="AX92" s="1"/>
-      <c r="AY92" s="1"/>
-      <c r="AZ92" s="1"/>
-      <c r="BA92" s="1"/>
-      <c r="BB92" s="1"/>
-      <c r="BC92" s="1"/>
-      <c r="BD92" s="1"/>
-      <c r="BE92" s="1"/>
-      <c r="BF92" s="1"/>
-      <c r="BG92" s="1"/>
-      <c r="BH92" s="1"/>
-      <c r="BI92" s="1"/>
-      <c r="BJ92" s="1"/>
-      <c r="BK92" s="1"/>
-      <c r="BL92" s="1"/>
-      <c r="BM92" s="1"/>
-      <c r="BN92" s="1"/>
-      <c r="BO92" s="1"/>
-      <c r="BP92" s="1"/>
-      <c r="BQ92" s="1"/>
-      <c r="BR92" s="1"/>
-      <c r="BS92" s="1"/>
-      <c r="BT92" s="1"/>
-      <c r="BU92" s="1"/>
-      <c r="BV92" s="1"/>
-      <c r="BW92" s="1"/>
-      <c r="BX92" s="1"/>
-      <c r="BY92" s="1"/>
-      <c r="BZ92" s="1"/>
-      <c r="CA92" s="1"/>
-      <c r="CB92" s="1"/>
-      <c r="CC92" s="1"/>
-      <c r="CD92" s="1"/>
-      <c r="CE92" s="1"/>
-      <c r="CF92" s="1"/>
-      <c r="CG92" s="1"/>
-      <c r="CH92" s="1"/>
-      <c r="CI92" s="1"/>
-      <c r="CJ92" s="1"/>
-      <c r="CK92" s="1"/>
-      <c r="CL92" s="1"/>
+      <c r="A92" s="1">
+        <v>0</v>
+      </c>
+      <c r="B92" s="2">
+        <v>0</v>
+      </c>
+      <c r="C92" s="2">
+        <v>0</v>
+      </c>
+      <c r="D92" s="2">
+        <v>0</v>
+      </c>
+      <c r="E92" s="2">
+        <v>0</v>
+      </c>
+      <c r="F92" s="2">
+        <v>0</v>
+      </c>
+      <c r="G92" s="2">
+        <v>0</v>
+      </c>
+      <c r="H92" s="2">
+        <v>0</v>
+      </c>
+      <c r="I92" s="2">
+        <v>0</v>
+      </c>
+      <c r="J92" s="2">
+        <v>0</v>
+      </c>
+      <c r="K92" s="2">
+        <v>0</v>
+      </c>
+      <c r="L92" s="2">
+        <v>0</v>
+      </c>
+      <c r="M92" s="2">
+        <v>0</v>
+      </c>
+      <c r="N92" s="2">
+        <v>0</v>
+      </c>
+      <c r="O92" s="2">
+        <v>0</v>
+      </c>
+      <c r="P92" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q92" s="2">
+        <v>0</v>
+      </c>
+      <c r="R92" s="2">
+        <v>0</v>
+      </c>
+      <c r="S92" s="2">
+        <v>0</v>
+      </c>
+      <c r="T92" s="2">
+        <v>0</v>
+      </c>
+      <c r="U92" s="2">
+        <v>0</v>
+      </c>
+      <c r="V92" s="2">
+        <v>0</v>
+      </c>
+      <c r="W92" s="2">
+        <v>0</v>
+      </c>
+      <c r="X92" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y92" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z92" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA92" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB92" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC92" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD92" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE92" s="2">
+        <v>0</v>
+      </c>
+      <c r="AF92" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG92" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH92" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI92" s="2">
+        <v>0</v>
+      </c>
+      <c r="AJ92" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK92" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL92" s="2">
+        <v>0</v>
+      </c>
+      <c r="AM92" s="2">
+        <v>0</v>
+      </c>
+      <c r="AN92" s="2">
+        <v>0</v>
+      </c>
+      <c r="AO92" s="2">
+        <v>0</v>
+      </c>
+      <c r="AP92" s="2">
+        <v>0</v>
+      </c>
+      <c r="AQ92" s="2">
+        <v>0</v>
+      </c>
+      <c r="AR92" s="2">
+        <v>0</v>
+      </c>
+      <c r="AS92" s="2">
+        <v>0</v>
+      </c>
+      <c r="AT92" s="2">
+        <v>0</v>
+      </c>
+      <c r="AU92" s="2">
+        <v>0</v>
+      </c>
+      <c r="AV92" s="2">
+        <v>0</v>
+      </c>
+      <c r="AW92" s="2">
+        <v>0</v>
+      </c>
+      <c r="AX92" s="2">
+        <v>0</v>
+      </c>
+      <c r="AY92" s="2">
+        <v>0</v>
+      </c>
+      <c r="AZ92" s="2">
+        <v>0</v>
+      </c>
+      <c r="BA92" s="2">
+        <v>0</v>
+      </c>
+      <c r="BB92" s="2">
+        <v>0</v>
+      </c>
+      <c r="BC92" s="2">
+        <v>0</v>
+      </c>
+      <c r="BD92" s="2">
+        <v>0</v>
+      </c>
+      <c r="BE92" s="2">
+        <v>0</v>
+      </c>
+      <c r="BF92" s="2">
+        <v>0</v>
+      </c>
+      <c r="BG92" s="2">
+        <v>0</v>
+      </c>
+      <c r="BH92" s="2">
+        <v>0</v>
+      </c>
+      <c r="BI92" s="2">
+        <v>0</v>
+      </c>
+      <c r="BJ92" s="2">
+        <v>0</v>
+      </c>
+      <c r="BK92" s="2">
+        <v>0</v>
+      </c>
+      <c r="BL92" s="2">
+        <v>0</v>
+      </c>
+      <c r="BM92" s="2">
+        <v>0</v>
+      </c>
+      <c r="BN92" s="2">
+        <v>0</v>
+      </c>
+      <c r="BO92" s="2">
+        <v>0</v>
+      </c>
+      <c r="BP92" s="2">
+        <v>0</v>
+      </c>
+      <c r="BQ92" s="2">
+        <v>0</v>
+      </c>
+      <c r="BR92" s="2">
+        <v>0</v>
+      </c>
+      <c r="BS92" s="2">
+        <v>0</v>
+      </c>
+      <c r="BT92" s="2">
+        <v>0</v>
+      </c>
+      <c r="BU92" s="2">
+        <v>0</v>
+      </c>
+      <c r="BV92" s="2">
+        <v>0</v>
+      </c>
+      <c r="BW92" s="2">
+        <v>0</v>
+      </c>
+      <c r="BX92" s="2">
+        <v>0</v>
+      </c>
+      <c r="BY92" s="2">
+        <v>0</v>
+      </c>
+      <c r="BZ92" s="2">
+        <v>0</v>
+      </c>
+      <c r="CA92" s="2">
+        <v>0</v>
+      </c>
+      <c r="CB92" s="2">
+        <v>0</v>
+      </c>
+      <c r="CC92" s="2">
+        <v>0</v>
+      </c>
+      <c r="CD92" s="2">
+        <v>0</v>
+      </c>
+      <c r="CE92" s="2">
+        <v>0</v>
+      </c>
+      <c r="CF92" s="2">
+        <v>0</v>
+      </c>
+      <c r="CG92" s="2">
+        <v>0</v>
+      </c>
+      <c r="CH92" s="2">
+        <v>0</v>
+      </c>
+      <c r="CI92" s="2">
+        <v>0</v>
+      </c>
+      <c r="CJ92" s="2">
+        <v>0</v>
+      </c>
+      <c r="CK92" s="2">
+        <v>0</v>
+      </c>
+      <c r="CL92" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="93" spans="1:90" x14ac:dyDescent="0.25">
       <c r="A93" s="1"/>
@@ -32460,7 +32913,7 @@
       <c r="CL179" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A3:CL90">
+  <conditionalFormatting sqref="A3:CL92">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>